<commit_message>
MEC identifiers version 2401
Update Monthly Enterprise Channel identifiers for version 2401 (Build 17231.20290)
</commit_message>
<xml_diff>
--- a/Microsoft 365/Monthly Enterprise Channel/accesscontrols.xlsx
+++ b/Microsoft 365/Monthly Enterprise Channel/accesscontrols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TcidDocs\MECOct2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TcidDocs\MECDec2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10A5C6E2-21C1-40ED-A364-A14150F92F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E53A3CE-C520-4794-8F5E-A3C9353D2F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5415" windowWidth="51600" windowHeight="15465"/>
+    <workbookView xWindow="2850" yWindow="4260" windowWidth="25470" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="accesscontrols" sheetId="1" r:id="rId1"/>

</xml_diff>